<commit_message>
Up icn and clinical stat
</commit_message>
<xml_diff>
--- a/Comparaison.xlsx
+++ b/Comparaison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23700" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="4380" yWindow="500" windowWidth="23700" windowHeight="16280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>xls</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>python</t>
+  </si>
+  <si>
+    <t>p10</t>
+  </si>
+  <si>
+    <t>p10bis</t>
   </si>
 </sst>
 </file>
@@ -445,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D48"/>
+  <dimension ref="A3:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="131" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,7 +497,7 @@
         <v>5.99</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" ref="D5:D21" si="0">(C5-B5)/B5</f>
+        <f t="shared" ref="D5:D23" si="0">(C5-B5)/B5</f>
         <v>-2.6016260162601647E-2</v>
       </c>
     </row>
@@ -683,11 +689,11 @@
         <v>3.72</v>
       </c>
       <c r="C18">
-        <v>2.89</v>
+        <v>3.07</v>
       </c>
       <c r="D18" s="6">
         <f t="shared" si="0"/>
-        <v>-0.22311827956989247</v>
+        <v>-0.17473118279569902</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -698,11 +704,11 @@
         <v>7.05</v>
       </c>
       <c r="C19">
-        <v>6.11</v>
+        <v>6.25</v>
       </c>
       <c r="D19" s="6">
         <f t="shared" si="0"/>
-        <v>-0.13333333333333328</v>
+        <v>-0.11347517730496452</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -736,333 +742,393 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="7">
-        <f>AVERAGE(B4:B21)</f>
-        <v>5.8605555555555551</v>
-      </c>
-      <c r="C22" s="7">
-        <f>AVERAGE(C4:C21)</f>
-        <v>5.7383333333333333</v>
-      </c>
-      <c r="D22" s="4">
-        <f>AVERAGE(D4:D21)</f>
-        <v>-3.4558591909864052E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>4.91</v>
+      </c>
+      <c r="C22">
+        <v>4.88</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
+        <v>-6.1099796334012722E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="C23">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="0"/>
+        <v>-2.6748971193415613E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="7">
+        <f>AVERAGE(B4:B23)</f>
+        <v>5.7629999999999999</v>
+      </c>
+      <c r="C24" s="7">
+        <f>AVERAGE(C4:C23)</f>
+        <v>5.6609999999999996</v>
+      </c>
+      <c r="D24" s="4">
+        <f>AVERAGE(D4:D23)</f>
+        <v>-2.9333417620090379E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26">
-        <v>5.18</v>
-      </c>
-      <c r="C26">
-        <v>6.15</v>
-      </c>
-      <c r="D26" s="5">
-        <f>(C26-B26)/B26</f>
-        <v>0.18725868725868738</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27">
-        <v>7.33</v>
-      </c>
-      <c r="C27">
-        <v>6.38</v>
-      </c>
-      <c r="D27" s="6">
-        <f t="shared" ref="D27:D34" si="1">(C27-B27)/B27</f>
-        <v>-0.12960436562073671</v>
-      </c>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>5.18</v>
+      </c>
+      <c r="C28">
+        <v>6.15</v>
+      </c>
+      <c r="D28" s="5">
+        <f>(C28-B28)/B28</f>
+        <v>0.18725868725868738</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>7.33</v>
+      </c>
+      <c r="C29">
+        <v>6.38</v>
+      </c>
+      <c r="D29" s="6">
+        <f t="shared" ref="D29:D37" si="1">(C29-B29)/B29</f>
+        <v>-0.12960436562073671</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>6</v>
       </c>
-      <c r="B28">
+      <c r="B30">
         <v>7.39</v>
       </c>
-      <c r="C28">
+      <c r="C30">
         <v>6.75</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D30" s="6">
         <f t="shared" si="1"/>
         <v>-8.66035182679296E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>8</v>
       </c>
-      <c r="B29">
+      <c r="B31">
         <v>5.6</v>
       </c>
-      <c r="C29">
+      <c r="C31">
         <v>6.79</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D31" s="5">
         <f t="shared" si="1"/>
         <v>0.21250000000000008</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>10</v>
       </c>
-      <c r="B30">
+      <c r="B32">
         <v>2.61</v>
       </c>
-      <c r="C30">
+      <c r="C32">
         <v>2.85</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D32" s="5">
         <f t="shared" si="1"/>
         <v>9.1954022988505829E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>12</v>
       </c>
-      <c r="B31">
+      <c r="B33">
         <v>6.15</v>
       </c>
-      <c r="C31">
+      <c r="C33">
         <v>9.33</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D33" s="5">
         <f t="shared" si="1"/>
         <v>0.51707317073170722</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>14</v>
       </c>
-      <c r="B32">
+      <c r="B34">
         <v>4.45</v>
       </c>
-      <c r="C32">
+      <c r="C34">
         <v>4.82</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D34" s="5">
         <f t="shared" si="1"/>
         <v>8.3146067415730357E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>16</v>
       </c>
-      <c r="B33">
+      <c r="B35">
         <v>3.72</v>
       </c>
-      <c r="C33">
+      <c r="C35">
         <v>7.05</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D35" s="5">
         <f t="shared" si="1"/>
         <v>0.89516129032258052</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>18</v>
       </c>
-      <c r="B34">
+      <c r="B36">
         <v>7.47</v>
       </c>
-      <c r="C34">
+      <c r="C36">
         <v>5.47</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D36" s="6">
         <f t="shared" si="1"/>
         <v>-0.2677376171352075</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="7">
-        <f>AVERAGE(B26:B34)</f>
-        <v>5.5444444444444443</v>
-      </c>
-      <c r="C35" s="7">
-        <f>AVERAGE(C26:C34)</f>
-        <v>6.1766666666666659</v>
-      </c>
-      <c r="D35" s="4">
-        <f>AVERAGE(D26:D34)</f>
-        <v>0.16701641529925973</v>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37">
+        <v>4.91</v>
+      </c>
+      <c r="C37">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="D37" s="6">
+        <f t="shared" si="1"/>
+        <v>-1.0183299389002001E-2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="7">
+        <f>AVERAGE(B28:B37)</f>
+        <v>5.4809999999999999</v>
+      </c>
+      <c r="C38" s="7">
+        <f>AVERAGE(C28:C37)</f>
+        <v>6.0449999999999999</v>
+      </c>
+      <c r="D38" s="4">
+        <f>AVERAGE(D28:D37)</f>
+        <v>0.14929644383043356</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39">
-        <v>5.41</v>
-      </c>
-      <c r="C39">
-        <v>5.99</v>
-      </c>
-      <c r="D39" s="5">
-        <f>(C39-B39)/B39</f>
-        <v>0.10720887245841036</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40">
-        <v>6.82</v>
-      </c>
-      <c r="C40">
-        <v>7.76</v>
-      </c>
-      <c r="D40" s="5">
-        <f t="shared" ref="D40:D47" si="2">(C40-B40)/B40</f>
-        <v>0.13782991202346034</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>6</v>
-      </c>
-      <c r="B41">
-        <v>6.9</v>
-      </c>
-      <c r="C41">
-        <v>8.9499999999999993</v>
-      </c>
-      <c r="D41" s="5">
-        <f t="shared" si="2"/>
-        <v>0.29710144927536214</v>
-      </c>
+      <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>5.41</v>
+      </c>
+      <c r="C42">
+        <v>5.99</v>
+      </c>
+      <c r="D42" s="5">
+        <f>(C42-B42)/B42</f>
+        <v>0.10720887245841036</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>6.82</v>
+      </c>
+      <c r="C43">
+        <v>7.76</v>
+      </c>
+      <c r="D43" s="5">
+        <f t="shared" ref="D43:D51" si="2">(C43-B43)/B43</f>
+        <v>0.13782991202346034</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44">
+        <v>6.9</v>
+      </c>
+      <c r="C44">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="D44" s="5">
+        <f t="shared" si="2"/>
+        <v>0.31159420289855078</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>8</v>
       </c>
-      <c r="B42">
+      <c r="B45">
         <v>4.8899999999999997</v>
       </c>
-      <c r="C42">
+      <c r="C45">
         <v>6.15</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D45" s="5">
         <f t="shared" si="2"/>
         <v>0.2576687116564419</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>10</v>
       </c>
-      <c r="B43">
+      <c r="B46">
         <v>2.1</v>
       </c>
-      <c r="C43">
+      <c r="C46">
         <v>2.33</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D46" s="5">
         <f t="shared" si="2"/>
         <v>0.10952380952380951</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>12</v>
       </c>
-      <c r="B44">
+      <c r="B47">
         <v>7.51</v>
       </c>
-      <c r="C44">
+      <c r="C47">
         <v>9.08</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D47" s="5">
         <f t="shared" si="2"/>
         <v>0.20905459387483361</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>14</v>
       </c>
-      <c r="B45">
+      <c r="B48">
         <v>4.22</v>
       </c>
-      <c r="C45">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="D45" s="5">
+      <c r="C48">
+        <v>4.97</v>
+      </c>
+      <c r="D48" s="5">
         <f t="shared" si="2"/>
-        <v>6.1611374407583103E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+        <v>0.17772511848341233</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>16</v>
       </c>
-      <c r="B46">
-        <v>2.89</v>
-      </c>
-      <c r="C46">
-        <v>6.11</v>
-      </c>
-      <c r="D46" s="5">
+      <c r="B49">
+        <v>3.07</v>
+      </c>
+      <c r="C49">
+        <v>6.25</v>
+      </c>
+      <c r="D49" s="5">
         <f t="shared" si="2"/>
-        <v>1.1141868512110726</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+        <v>1.0358306188925082</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>18</v>
       </c>
-      <c r="B47">
+      <c r="B50">
         <v>6.18</v>
       </c>
-      <c r="C47">
+      <c r="C50">
         <v>5.52</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D50" s="6">
         <f t="shared" si="2"/>
         <v>-0.10679611650485439</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="7">
-        <f>AVERAGE(B39:B47)</f>
-        <v>5.2133333333333338</v>
-      </c>
-      <c r="C48" s="7">
-        <f>AVERAGE(C39:C47)</f>
-        <v>6.2633333333333319</v>
-      </c>
-      <c r="D48" s="4">
-        <f>AVERAGE(D39:D47)</f>
-        <v>0.24304327310290214</v>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51">
+        <v>4.88</v>
+      </c>
+      <c r="C51">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="D51" s="6">
+        <f t="shared" si="2"/>
+        <v>-3.0737704918032679E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="7">
+        <f>AVERAGE(B42:B51)</f>
+        <v>5.1980000000000004</v>
+      </c>
+      <c r="C52" s="7">
+        <f>AVERAGE(C42:C51)</f>
+        <v>6.1829999999999998</v>
+      </c>
+      <c r="D52" s="4">
+        <f>AVERAGE(D42:D51)</f>
+        <v>0.22089020183885402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>